<commit_message>
Updated .xlsx file with results from Feb 17th, 2022.
</commit_message>
<xml_diff>
--- a/Results_Summary.xlsx
+++ b/Results_Summary.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garibotti/Desktop/Radiacao_Resultados_Fev_22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garibotti/Desktop/Radiacao_Resultados_Fev_22/radiation_feb_22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566CB863-3001-4640-84CC-D229B8EF075E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC35F0E3-5A6B-7B47-8B65-642AF08F3A43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="500" windowWidth="22900" windowHeight="13920" xr2:uid="{90D526D0-F929-254D-966D-C6E626311E84}"/>
+    <workbookView xWindow="4580" yWindow="1660" windowWidth="22900" windowHeight="9500" activeTab="1" xr2:uid="{90D526D0-F929-254D-966D-C6E626311E84}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="8jpg_yolov5_on_cX_in_sequence" sheetId="1" r:id="rId1"/>
+    <sheet name="7jpg_yolov5_on_cX" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
   <si>
     <t>Total</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>February 9th, 2022</t>
+  </si>
+  <si>
+    <t>February 17th, 2022</t>
   </si>
 </sst>
 </file>
@@ -208,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +231,9 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -560,25 +567,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942BB48D-C9B9-944D-8C94-74735C4CBEBD}">
   <dimension ref="C3:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C3" s="4"/>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C4" s="4"/>
@@ -744,17 +751,17 @@
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C10" s="4"/>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C11" s="4"/>
@@ -920,17 +927,17 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" s="4"/>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" s="4"/>
@@ -1102,4 +1109,182 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876B9EAF-1DB9-5445-AA0D-84EA29E6CED4}">
+  <dimension ref="B2:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="4"/>
+      <c r="C2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="4"/>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1">
+        <v>78</v>
+      </c>
+      <c r="E4" s="1">
+        <v>78</v>
+      </c>
+      <c r="F4" s="1">
+        <v>77</v>
+      </c>
+      <c r="G4" s="1">
+        <v>77</v>
+      </c>
+      <c r="H4" s="1">
+        <v>77</v>
+      </c>
+      <c r="I4" s="1">
+        <v>79</v>
+      </c>
+      <c r="J4" s="5">
+        <f>SUM(C4:I4)</f>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1">
+        <v>49</v>
+      </c>
+      <c r="F5" s="1">
+        <v>52</v>
+      </c>
+      <c r="G5" s="1">
+        <v>51</v>
+      </c>
+      <c r="H5" s="1">
+        <v>50</v>
+      </c>
+      <c r="I5" s="1">
+        <v>50</v>
+      </c>
+      <c r="J5" s="6">
+        <f>SUM(C5:I5)/J4</f>
+        <v>0.65321100917431196</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <f>SUM(C6:I6)/J4</f>
+        <v>1.4678899082568808E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1">
+        <v>29</v>
+      </c>
+      <c r="J7" s="6">
+        <f>SUM(C7:I7)/J4</f>
+        <v>0.33211009174311928</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>